<commit_message>
Atualização RDD 10 - Liga Eliminação
Ajuste e atualização da pontuação da Rodada 10 na Liga Eliminação.
</commit_message>
<xml_diff>
--- a/liga_eliminacao/datasets_liga_eliminacao/Jogadores_Mais_Escalados_Por_Posicao_Liga_Eliminacao.xlsx
+++ b/liga_eliminacao/datasets_liga_eliminacao/Jogadores_Mais_Escalados_Por_Posicao_Liga_Eliminacao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>Nome</t>
   </si>
@@ -40,15 +40,15 @@
     <t>Léo Ortiz</t>
   </si>
   <si>
+    <t>Pedro Henrique</t>
+  </si>
+  <si>
     <t>Ignácio</t>
   </si>
   <si>
     <t>Junior Alonso</t>
   </si>
   <si>
-    <t>Vitão</t>
-  </si>
-  <si>
     <t>Juninho Capixaba</t>
   </si>
   <si>
@@ -70,12 +70,12 @@
     <t>Alan Patrick</t>
   </si>
   <si>
+    <t>Jhon Jhon</t>
+  </si>
+  <si>
     <t>Rubens</t>
   </si>
   <si>
-    <t>Jhon Jhon</t>
-  </si>
-  <si>
     <t>Yuri Alberto</t>
   </si>
   <si>
@@ -85,6 +85,9 @@
     <t>Igor Jesus</t>
   </si>
   <si>
+    <t>Eduardo Sasha</t>
+  </si>
+  <si>
     <t>Estêvão</t>
   </si>
   <si>
@@ -115,13 +118,13 @@
     <t>FLA</t>
   </si>
   <si>
+    <t>RBB</t>
+  </si>
+  <si>
     <t>FLU</t>
   </si>
   <si>
     <t>CAM</t>
-  </si>
-  <si>
-    <t>RBB</t>
   </si>
   <si>
     <t>SAN</t>
@@ -513,13 +516,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -527,13 +530,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -541,10 +544,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>31</v>
@@ -555,13 +558,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -569,13 +572,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -583,13 +586,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -597,13 +600,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D8">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -611,13 +614,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -625,13 +628,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -639,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>42</v>
@@ -653,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>34</v>
@@ -667,13 +670,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13">
-        <v>129</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -681,13 +684,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -695,13 +698,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -709,13 +712,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
       <c r="D16">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -723,13 +726,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -737,13 +740,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -751,13 +754,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -765,10 +768,10 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20">
         <v>55</v>
@@ -776,30 +779,30 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D21">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D22">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>